<commit_message>
final charts and readme
</commit_message>
<xml_diff>
--- a/1608_google_autonomous.xlsx
+++ b/1608_google_autonomous.xlsx
@@ -68,9 +68,6 @@
     <t>% A</t>
   </si>
   <si>
-    <t>miles / veh-day</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>A miles Per week</t>
+  </si>
+  <si>
+    <t>A miles / veh-day</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,10 +514,10 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>9</v>
@@ -526,7 +526,7 @@
         <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -574,7 +574,7 @@
         <v>228366.6451612903</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O2" s="6">
         <f t="shared" ref="O2:O14" si="2">I2/(I2+J2)</f>

</xml_diff>